<commit_message>
Changed file output encoding and added annotations.
File output now supports more characters (e.g. μ) in .csv files opened by Microsoft Excel.
</commit_message>
<xml_diff>
--- a/examples/EZIO_input_template.xlsx
+++ b/examples/EZIO_input_template.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel Sandborn\Google Drive\GitStuff\PyCO2SYS\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DA7E1D1-F596-49B1-88DA-3105CB4A2AC7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ABEDC81-32BA-4129-B4FC-694AC49741BC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="-5325" windowWidth="19440" windowHeight="15000" xr2:uid="{8D57C8EA-B6B7-45E3-9787-7AE55EB3EF22}"/>
+    <workbookView xWindow="-13995" yWindow="1995" windowWidth="13215" windowHeight="8970" xr2:uid="{8D57C8EA-B6B7-45E3-9787-7AE55EB3EF22}"/>
   </bookViews>
   <sheets>
     <sheet name="DATA" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -448,7 +448,7 @@
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -574,7 +574,7 @@
         <v>2226.38</v>
       </c>
       <c r="J5">
-        <v>7.8590002059936523</v>
+        <v>7.8649997711181641</v>
       </c>
     </row>
   </sheetData>

</xml_diff>